<commit_message>
add frontend and fix backend
</commit_message>
<xml_diff>
--- a/documents-lending/hired-workers/employment/vipiska-test-5.xlsx
+++ b/documents-lending/hired-workers/employment/vipiska-test-5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java-Spring\bank-lending-system\documents-lending\employment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java-Spring\bank-lending-system\documents-lending\hired-workers\employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D5C318-976D-4B16-89C4-F62E397DA2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5589C5-6F23-4262-84AB-AC99B324D899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="4065" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4425" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -204,15 +204,9 @@
     <t>менеджер по продажам</t>
   </si>
   <si>
-    <t>Попов</t>
-  </si>
-  <si>
     <t xml:space="preserve">Максим </t>
   </si>
   <si>
-    <t>Анатольевич</t>
-  </si>
-  <si>
     <t>ООО "Арбалет"</t>
   </si>
   <si>
@@ -220,6 +214,12 @@
   </si>
   <si>
     <t>Главный Лиханов</t>
+  </si>
+  <si>
+    <t>Ковалев</t>
+  </si>
+  <si>
+    <t>Иванович</t>
   </si>
 </sst>
 </file>
@@ -563,6 +563,72 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -577,72 +643,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,7 +930,7 @@
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="C14" sqref="C14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,107 +957,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
     </row>
     <row r="5" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1070,7 +1070,7 @@
       <c r="M5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="60">
+      <c r="N5" s="36">
         <v>41961</v>
       </c>
       <c r="O5" s="5"/>
@@ -1081,10 +1081,10 @@
       <c r="T5" s="5"/>
     </row>
     <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1098,7 +1098,7 @@
       <c r="M6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="61">
+      <c r="N6" s="37">
         <v>124578</v>
       </c>
       <c r="O6" s="5"/>
@@ -1109,22 +1109,22 @@
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
     </row>
     <row r="8" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="D8" s="6"/>
@@ -1150,15 +1150,15 @@
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
+      <c r="B11" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1170,15 +1170,15 @@
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
+      <c r="B12" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1187,18 +1187,18 @@
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1207,14 +1207,14 @@
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="56">
-        <v>32872</v>
-      </c>
-      <c r="D14" s="54"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53">
+        <v>30335</v>
+      </c>
+      <c r="D14" s="51"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -1237,19 +1237,19 @@
       <c r="B16" s="7"/>
     </row>
     <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
@@ -1266,16 +1266,16 @@
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="54">
+      <c r="B18" s="51">
         <v>6789012345</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -1307,15 +1307,15 @@
       <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="12"/>
       <c r="I21" s="33">
         <v>45695</v>
@@ -1327,9 +1327,9 @@
       <c r="I22" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
     </row>
     <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -1361,9 +1361,9 @@
       <c r="I24" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
@@ -1402,13 +1402,13 @@
       <c r="L28" s="47"/>
       <c r="M28" s="47"/>
       <c r="N28" s="47"/>
-      <c r="O28" s="45" t="s">
+      <c r="O28" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="48"/>
       <c r="T28" s="26"/>
     </row>
     <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1434,11 +1434,11 @@
       </c>
       <c r="M29" s="47"/>
       <c r="N29" s="47"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
+      <c r="O29" s="48"/>
+      <c r="P29" s="48"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="48"/>
+      <c r="S29" s="48"/>
       <c r="T29" s="26"/>
     </row>
     <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1468,11 +1468,11 @@
       <c r="N30" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="48"/>
+      <c r="S30" s="48"/>
       <c r="T30" s="26"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1483,18 +1483,18 @@
       <c r="E31" s="46"/>
       <c r="F31" s="46"/>
       <c r="G31" s="46"/>
-      <c r="H31" s="48"/>
+      <c r="H31" s="49"/>
       <c r="I31" s="46"/>
       <c r="J31" s="46"/>
       <c r="K31" s="46"/>
       <c r="L31" s="46"/>
       <c r="M31" s="46"/>
       <c r="N31" s="46"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
       <c r="T31" s="26"/>
     </row>
     <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1505,7 +1505,7 @@
       <c r="E32" s="46"/>
       <c r="F32" s="46"/>
       <c r="G32" s="46"/>
-      <c r="H32" s="48"/>
+      <c r="H32" s="49"/>
       <c r="I32" s="46"/>
       <c r="J32" s="46"/>
       <c r="K32" s="46"/>
@@ -1516,11 +1516,11 @@
       <c r="N32" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
+      <c r="O32" s="48"/>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
+      <c r="S32" s="48"/>
       <c r="T32" s="26"/>
     </row>
     <row r="33" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1531,44 +1531,44 @@
       <c r="E33" s="46"/>
       <c r="F33" s="46"/>
       <c r="G33" s="46"/>
-      <c r="H33" s="48"/>
+      <c r="H33" s="49"/>
       <c r="I33" s="46"/>
       <c r="J33" s="46"/>
       <c r="K33" s="46"/>
       <c r="L33" s="46"/>
       <c r="M33" s="46"/>
       <c r="N33" s="46"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
+      <c r="O33" s="48"/>
+      <c r="P33" s="48"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="48"/>
       <c r="T33" s="26"/>
     </row>
     <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27">
         <v>1</v>
       </c>
-      <c r="B34" s="50">
+      <c r="B34" s="42">
         <v>2</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="27">
         <v>3</v>
       </c>
-      <c r="F34" s="50">
+      <c r="F34" s="42">
         <v>4</v>
       </c>
-      <c r="G34" s="50"/>
+      <c r="G34" s="42"/>
       <c r="H34" s="27">
         <v>5</v>
       </c>
-      <c r="I34" s="50">
+      <c r="I34" s="42">
         <v>6</v>
       </c>
-      <c r="J34" s="50"/>
-      <c r="K34" s="50"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
       <c r="L34" s="27">
         <v>7</v>
       </c>
@@ -1578,34 +1578,34 @@
       <c r="N34" s="27">
         <v>9</v>
       </c>
-      <c r="O34" s="51">
+      <c r="O34" s="38">
         <v>10</v>
       </c>
-      <c r="P34" s="51"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="51"/>
-      <c r="S34" s="51"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="38"/>
+      <c r="S34" s="38"/>
     </row>
     <row r="35" spans="1:20" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="49">
+      <c r="B35" s="44">
         <v>41961</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
       <c r="E35" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="50" t="s">
+      <c r="F35" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="G35" s="50"/>
+      <c r="G35" s="42"/>
       <c r="H35" s="27"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
       <c r="L35" s="27" t="s">
         <v>45</v>
       </c>
@@ -1615,33 +1615,33 @@
       <c r="N35" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="O35" s="51"/>
-      <c r="P35" s="51"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="51"/>
-      <c r="S35" s="51"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
+      <c r="S35" s="38"/>
       <c r="T35" s="28"/>
     </row>
     <row r="36" spans="1:20" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
       <c r="E36" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
       <c r="H36" s="27"/>
-      <c r="I36" s="50" t="s">
+      <c r="I36" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="J36" s="50"/>
-      <c r="K36" s="50"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="42"/>
       <c r="L36" s="27" t="s">
         <v>45</v>
       </c>
@@ -1651,33 +1651,33 @@
       <c r="N36" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="O36" s="51"/>
-      <c r="P36" s="51"/>
-      <c r="Q36" s="51"/>
-      <c r="R36" s="51"/>
-      <c r="S36" s="51"/>
+      <c r="O36" s="38"/>
+      <c r="P36" s="38"/>
+      <c r="Q36" s="38"/>
+      <c r="R36" s="38"/>
+      <c r="S36" s="38"/>
       <c r="T36" s="28"/>
     </row>
     <row r="37" spans="1:20" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="49">
+      <c r="B37" s="44">
         <v>43344</v>
       </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="50" t="s">
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="G37" s="50"/>
+      <c r="G37" s="42"/>
       <c r="H37" s="27"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
       <c r="L37" s="27" t="s">
         <v>45</v>
       </c>
@@ -1687,18 +1687,18 @@
       <c r="N37" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="O37" s="51"/>
-      <c r="P37" s="51"/>
-      <c r="Q37" s="51"/>
-      <c r="R37" s="51"/>
-      <c r="S37" s="51"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="38"/>
+      <c r="R37" s="38"/>
+      <c r="S37" s="38"/>
     </row>
     <row r="38" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
+      <c r="A38" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
       <c r="E38" s="29"/>
       <c r="G38" s="29"/>
       <c r="H38" s="34" t="s">
@@ -1707,11 +1707,11 @@
       <c r="I38" s="29"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
       <c r="D39" s="30"/>
       <c r="E39" s="30" t="s">
         <v>36</v>
@@ -1734,10 +1734,10 @@
       <c r="K40" s="32"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="58">
+      <c r="A41" s="40">
         <v>45680</v>
       </c>
-      <c r="B41" s="59"/>
+      <c r="B41" s="41"/>
       <c r="I41" s="32" t="s">
         <v>40</v>
       </c>
@@ -1750,6 +1750,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="C2:T2"/>
+    <mergeCell ref="A3:T3"/>
+    <mergeCell ref="A4:T4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="A7:N7"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="O28:S33"/>
+    <mergeCell ref="B29:D33"/>
+    <mergeCell ref="E29:E33"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="F30:G33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="I30:K33"/>
+    <mergeCell ref="L30:L33"/>
+    <mergeCell ref="M30:M33"/>
+    <mergeCell ref="N30:N33"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="B28:N28"/>
     <mergeCell ref="O37:S37"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A41:B41"/>
@@ -1766,42 +1802,6 @@
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="O36:S36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="B28:N28"/>
-    <mergeCell ref="O28:S33"/>
-    <mergeCell ref="B29:D33"/>
-    <mergeCell ref="E29:E33"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="F30:G33"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="I30:K33"/>
-    <mergeCell ref="L30:L33"/>
-    <mergeCell ref="M30:M33"/>
-    <mergeCell ref="N30:N33"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="A7:N7"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="C2:T2"/>
-    <mergeCell ref="A3:T3"/>
-    <mergeCell ref="A4:T4"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="68" orientation="landscape" r:id="rId1"/>

</xml_diff>